<commit_message>
Almost everything blocked in
</commit_message>
<xml_diff>
--- a/Washing Machine Design Calculations.xlsx
+++ b/Washing Machine Design Calculations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tommy Rohmann\OneDrive\Projects\Microgravity-Press-Washing-Machine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dcdf7eb514dfaeec/Projects/Microgravity-Press-Washing-Machine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D766C26B-1EE4-490E-9437-84C4703C55A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="13_ncr:1_{D766C26B-1EE4-490E-9437-84C4703C55A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73C9E0BE-9C8D-449A-AA26-FEBA4B6F3122}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="17115" windowHeight="10755" activeTab="1" xr2:uid="{73A7591B-B5CA-4318-9343-9B3FDBEBCAB4}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="17115" windowHeight="10755" firstSheet="1" activeTab="3" xr2:uid="{73A7591B-B5CA-4318-9343-9B3FDBEBCAB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Design and Material Specs" sheetId="2" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="350">
   <si>
     <t>Desired Force Application</t>
   </si>
@@ -833,9 +833,6 @@
     <t>Minimum Pin Diameter for Shear Stress</t>
   </si>
   <si>
-    <t>Required Pin Thickness (for hatch beam)</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
@@ -947,12 +944,6 @@
     <t>Stress at Location</t>
   </si>
   <si>
-    <t>SuperStructure</t>
-  </si>
-  <si>
-    <t>Access hatch and conduit</t>
-  </si>
-  <si>
     <t>Known based on component sizing</t>
   </si>
   <si>
@@ -1112,16 +1103,37 @@
     <t>in3</t>
   </si>
   <si>
-    <t>Area of Space</t>
-  </si>
-  <si>
-    <t>Cross Sectional Area of Beam</t>
-  </si>
-  <si>
-    <t>Stress Due to Tension</t>
-  </si>
-  <si>
     <t>Top Bearing Thickness</t>
+  </si>
+  <si>
+    <t>Strut Thickness</t>
+  </si>
+  <si>
+    <t>Strut Width</t>
+  </si>
+  <si>
+    <t>Hole Diameter</t>
+  </si>
+  <si>
+    <t>Pin Cross Section Area</t>
+  </si>
+  <si>
+    <t>Holding Pin Calcs</t>
+  </si>
+  <si>
+    <t>Check Strut Cross Section</t>
+  </si>
+  <si>
+    <t>Pin Cross Section Area for Shear</t>
+  </si>
+  <si>
+    <t>Stress</t>
+  </si>
+  <si>
+    <t>Strut Cross Section Area at Hole</t>
+  </si>
+  <si>
+    <t>Width</t>
   </si>
 </sst>
 </file>
@@ -1436,7 +1448,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1505,6 +1517,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1674,50 +1687,6 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>609781</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>58118</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="4678949" cy="1484096"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B84E5AE-7496-4690-BB9E-CD18C7C0FD5E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm rot="16200000">
-          <a:off x="2207208" y="1375341"/>
-          <a:ext cx="1484096" cy="4678949"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2088,7 +2057,7 @@
         <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="M4" t="s">
         <v>9</v>
@@ -2248,7 +2217,7 @@
     </row>
     <row r="16" spans="3:17" x14ac:dyDescent="0.45">
       <c r="M16" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N16">
         <v>4.4482220000000003</v>
@@ -2446,7 +2415,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F7F30C8-AEF8-4367-97CA-93B5B12A08F4}">
   <dimension ref="A1:AI56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
@@ -2486,7 +2455,7 @@
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
       <c r="P2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.45">
@@ -2561,7 +2530,7 @@
       </c>
       <c r="N4" s="5"/>
       <c r="P4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="Q4" s="1">
         <f>L5</f>
@@ -2571,7 +2540,7 @@
         <v>103</v>
       </c>
       <c r="S4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="W4" s="46"/>
       <c r="X4" s="46"/>
@@ -2619,14 +2588,14 @@
       <c r="Y5" s="49"/>
       <c r="Z5" s="46"/>
       <c r="AA5" s="47" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="AB5" s="48"/>
       <c r="AC5" s="48"/>
       <c r="AD5" s="49"/>
       <c r="AE5" s="46"/>
       <c r="AF5" s="47" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="AG5" s="48"/>
       <c r="AH5" s="48"/>
@@ -3049,7 +3018,7 @@
         <v>34800</v>
       </c>
       <c r="X12" s="21" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="Y12" s="22"/>
       <c r="Z12" s="46"/>
@@ -3097,7 +3066,7 @@
         <v>8.5488505747126436E-2</v>
       </c>
       <c r="X13" s="51" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="Y13" s="52"/>
       <c r="Z13" s="46"/>
@@ -3207,7 +3176,7 @@
       <c r="Y16" s="46"/>
       <c r="Z16" s="46"/>
       <c r="AA16" s="46" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AB16" s="46"/>
       <c r="AC16" s="46"/>
@@ -3244,7 +3213,7 @@
       <c r="Y17" s="49"/>
       <c r="Z17" s="46"/>
       <c r="AA17" s="47" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="AB17" s="48"/>
       <c r="AC17" s="48"/>
@@ -3302,7 +3271,7 @@
       <c r="Y19" s="22"/>
       <c r="Z19" s="46"/>
       <c r="AA19" s="13" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="AB19" s="21">
         <f>0.125</f>
@@ -3392,7 +3361,7 @@
       <c r="Y22" s="22"/>
       <c r="Z22" s="46"/>
       <c r="AA22" s="13" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="AB22" s="21">
         <f>AB21*AppliedForceNormal*0.5/(2*AB19*AB20)</f>
@@ -3421,7 +3390,7 @@
       <c r="Y23" s="52"/>
       <c r="Z23" s="46"/>
       <c r="AA23" s="50" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="AB23" s="51">
         <v>0.25</v>
@@ -3442,7 +3411,7 @@
       <c r="Y24" s="46"/>
       <c r="Z24" s="46"/>
       <c r="AA24" s="53" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="AB24" s="46">
         <f>W23+(2*AB23)</f>
@@ -3501,7 +3470,7 @@
         <v>152</v>
       </c>
       <c r="F29" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G29">
         <f>B34/(B30/12)</f>
@@ -3544,7 +3513,7 @@
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A32" s="10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B32" s="5">
         <v>1.25</v>
@@ -3619,7 +3588,7 @@
     </row>
     <row r="40" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="F40" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -3737,7 +3706,7 @@
         <v>6.873996997881</v>
       </c>
       <c r="C46" s="34" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D46" s="30"/>
       <c r="F46" s="10" t="s">
@@ -3780,7 +3749,7 @@
         <v>50</v>
       </c>
       <c r="E50" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.45">
@@ -3789,10 +3758,10 @@
         <v>5.2359877559829888</v>
       </c>
       <c r="E51" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F51" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.45">
@@ -3801,7 +3770,7 @@
         <v>6.873996997881</v>
       </c>
       <c r="E52" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.45">
@@ -3810,7 +3779,7 @@
         <v>35.992164115568741</v>
       </c>
       <c r="E53" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F53">
         <f>0.105*90*B46</f>
@@ -3822,7 +3791,7 @@
         <v>24</v>
       </c>
       <c r="E55" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.45">
@@ -3831,7 +3800,7 @@
         <v>1.4996735048153642</v>
       </c>
       <c r="E56" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F56">
         <f>6000*0.224808943</f>
@@ -3934,7 +3903,7 @@
       </c>
       <c r="D4" s="11"/>
       <c r="F4" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G4" s="5">
         <f>B12</f>
@@ -3945,7 +3914,7 @@
       </c>
       <c r="I4" s="5"/>
       <c r="K4" s="10" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L4" s="5">
         <v>0.75</v>
@@ -3977,7 +3946,7 @@
       </c>
       <c r="I5" s="5"/>
       <c r="K5" s="10" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L5" s="5">
         <f>(L4^2)*PI()</f>
@@ -4038,7 +4007,7 @@
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="K7" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L7" s="34">
         <f>L6/L5</f>
@@ -4352,7 +4321,7 @@
       <c r="R24" s="5"/>
       <c r="S24" s="5"/>
       <c r="U24" s="10" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="V24" s="5">
         <f>3/8</f>
@@ -4401,7 +4370,7 @@
       <c r="R25" s="5"/>
       <c r="S25" s="5"/>
       <c r="U25" s="10" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="V25" s="5">
         <f>(V24^2)*PI()</f>
@@ -4496,7 +4465,7 @@
       <c r="R27" s="5"/>
       <c r="S27" s="5"/>
       <c r="U27" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="V27" s="34">
         <f>V26/V25</f>
@@ -4729,7 +4698,7 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.45">
@@ -4807,7 +4776,7 @@
       </c>
       <c r="I44" s="5"/>
       <c r="K44" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="L44" s="5">
         <v>1</v>
@@ -4829,7 +4798,7 @@
         <v>71</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>239</v>
@@ -4989,929 +4958,330 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58B192C6-AACC-4DBA-B547-B2E0428B8816}">
-  <dimension ref="A5:O77"/>
+  <dimension ref="A2:H33"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
+    <col min="1" max="1" width="21.796875" customWidth="1"/>
     <col min="2" max="2" width="26.59765625" customWidth="1"/>
     <col min="7" max="7" width="26" customWidth="1"/>
     <col min="12" max="12" width="32.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B5" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="G5" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="L5" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B6" s="5"/>
-      <c r="C6" s="5" t="s">
-        <v>14</v>
+    <row r="2" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B3" s="31"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="33"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B4" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.125</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="11"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B5" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="11"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B6" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="C6">
+        <f>C5*C4</f>
+        <v>0.125</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B7" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="C7" s="5">
+        <v>162</v>
+      </c>
+      <c r="E6" s="11"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B7" s="10" t="s">
+        <v>347</v>
+      </c>
+      <c r="C7">
+        <f>C18/C6</f>
+        <v>4800</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="11"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <f>C17/C7</f>
+        <v>7.25</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="11"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>344</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>342</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="11"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B10" s="10" t="s">
+        <v>343</v>
+      </c>
+      <c r="C10" s="5">
+        <f>C4*C9</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="11"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B11" s="54" t="s">
+        <v>347</v>
+      </c>
+      <c r="C11">
+        <f>C18/C10</f>
+        <v>19200</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="11"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B12" s="54" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <f>C17/C11</f>
+        <v>1.8125</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="11"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>345</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>346</v>
+      </c>
+      <c r="C13">
+        <f>(C9/2)^2*PI()</f>
+        <v>4.9087385212340517E-2</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="11"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B14" s="10"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="11"/>
+    </row>
+    <row r="15" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B15" s="23" t="s">
+        <v>348</v>
+      </c>
+      <c r="C15">
+        <f>C6-C10</f>
+        <v>9.375E-2</v>
+      </c>
+      <c r="D15" s="34"/>
+      <c r="E15" s="30"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="C17" s="5">
+        <f>SS303FatigueStrength</f>
+        <v>34800</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="C18" s="5">
         <f>AppliedForceNormal</f>
         <v>600</v>
       </c>
-      <c r="D7" s="5" t="s">
+    </row>
+    <row r="23" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B23" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B24" s="31" t="s">
+        <v>267</v>
+      </c>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="33"/>
+      <c r="G24" t="s">
+        <v>349</v>
+      </c>
+      <c r="H24">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B25" s="10"/>
+      <c r="C25" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="G25" t="s">
+        <v>301</v>
+      </c>
+      <c r="H25">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B26" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="C26" s="5">
+        <v>200</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="G7" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="H7" s="5">
-        <v>0.25</v>
-      </c>
-      <c r="I7" s="5" t="s">
+      <c r="E26" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="G26" t="s">
+        <v>228</v>
+      </c>
+      <c r="H26">
+        <f>(H24*H25^2)/6</f>
+        <v>0.12760416666666666</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B27" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="C27" s="5">
+        <f>AppliedForceNormal+C26</f>
+        <v>800</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E27" s="11"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B28" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="C28" s="5">
+        <f>MachineWidth-0.25</f>
+        <v>8.25</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="J7" s="5"/>
-      <c r="L7" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="M7" s="5">
-        <v>1</v>
-      </c>
-      <c r="N7" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="O7" s="5"/>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B8" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="C8" s="5">
-        <f>3.725*2</f>
-        <v>7.45</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>289</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="H8" s="5">
+      <c r="E28" s="11" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B29" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="C29" s="5">
+        <f>C27/2</f>
+        <v>400</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E29" s="11"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B30" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="C30" s="5">
+        <f>C29*C28/2</f>
+        <v>1650</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="E30" s="11"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B31" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="5">
         <v>2</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="D31" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="5"/>
-      <c r="L8" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="M8" s="5">
+      <c r="E31" s="11"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B32" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="C32" s="5">
         <f>SS303FatigueStrength</f>
         <v>34800</v>
       </c>
-      <c r="N8" s="5" t="s">
+      <c r="D32" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="O8" s="5"/>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B9" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="C9" s="5">
-        <f>C7/2</f>
-        <v>300</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="E9" s="5"/>
-      <c r="G9" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="H9" s="5">
-        <f>H7*H8</f>
-        <v>0.5</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="J9" s="5"/>
-      <c r="L9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M9" s="5">
-        <v>5</v>
-      </c>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B10" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C10" s="5">
-        <f>C9*C8/2</f>
-        <v>1117.5</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="E10" s="5"/>
-      <c r="G10" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="H10" s="5">
-        <f>SQRT((6*C13)/H9)</f>
-        <v>0.87788931829269556</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="J10" s="5"/>
-      <c r="L10" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="M10" s="5">
-        <f>AppliedForceNormal*M9/(M8*M7)</f>
-        <v>8.6206896551724144E-2</v>
-      </c>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="5">
-        <v>2</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="L11" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="M11" s="5">
-        <v>0.25</v>
-      </c>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B12" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="C12" s="5">
-        <f>SS303FatigueStrength</f>
-        <v>34800</v>
-      </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="L12" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="M12" s="5">
-        <f>(((M7/2)^2)*PI())-(M7*M11)</f>
-        <v>0.53539816339744828</v>
-      </c>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B13" s="5" t="s">
+      <c r="E32" s="11"/>
+    </row>
+    <row r="33" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B33" s="23" t="s">
         <v>240</v>
       </c>
-      <c r="C13" s="5">
-        <f>C10*C11/C12</f>
-        <v>6.4224137931034486E-2</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="L13" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="M13" s="5">
-        <f>AppliedForceNormal/M12</f>
-        <v>1120.6612966182238</v>
-      </c>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B16" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C17" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="D18">
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="D19">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="D20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="D21">
-        <f>D20*D18*2</f>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="D22">
-        <f>D19*D18</f>
-        <v>1.0625</v>
-      </c>
-    </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C23" t="s">
-        <v>343</v>
-      </c>
-      <c r="D23">
-        <f>D21+D22</f>
-        <v>1.3125</v>
-      </c>
-    </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C24" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="C36" s="3"/>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="C37" s="3"/>
-    </row>
-    <row r="38" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A38" t="s">
-        <v>288</v>
-      </c>
-      <c r="B38" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="B39" s="31" t="s">
-        <v>268</v>
-      </c>
-      <c r="C39" s="32"/>
-      <c r="D39" s="32"/>
-      <c r="E39" s="33"/>
-      <c r="G39" s="31" t="s">
-        <v>267</v>
-      </c>
-      <c r="H39" s="32"/>
-      <c r="I39" s="32"/>
-      <c r="J39" s="33"/>
-      <c r="L39" s="31" t="s">
-        <v>249</v>
-      </c>
-      <c r="M39" s="32"/>
-      <c r="N39" s="32"/>
-      <c r="O39" s="33"/>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="B40" s="10"/>
-      <c r="C40" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E40" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="G40" s="10"/>
-      <c r="H40" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I40" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="J40" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="L40" s="10"/>
-      <c r="M40" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="N40" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="O40" s="11" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="B41" s="10" t="s">
-        <v>269</v>
-      </c>
-      <c r="C41" s="5">
-        <v>200</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="E41" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="G41" s="10" t="s">
-        <v>238</v>
-      </c>
-      <c r="H41" s="27">
-        <v>0.5</v>
-      </c>
-      <c r="I41" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="J41" s="11"/>
-      <c r="L41" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="M41" s="5">
-        <f>C42</f>
-        <v>800</v>
-      </c>
-      <c r="N41" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="O41" s="11"/>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="B42" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="C42" s="5">
-        <f>AppliedForceNormal+C41</f>
-        <v>800</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="E42" s="11"/>
-      <c r="G42" s="10" t="s">
-        <v>239</v>
-      </c>
-      <c r="H42" s="27">
-        <v>2</v>
-      </c>
-      <c r="I42" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J42" s="11"/>
-      <c r="L42" s="10" t="s">
-        <v>246</v>
-      </c>
-      <c r="M42" s="5">
-        <f>H43</f>
-        <v>1</v>
-      </c>
-      <c r="N42" s="5"/>
-      <c r="O42" s="11"/>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="B43" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="C43" s="5">
-        <f>MachineWidth-0.25</f>
-        <v>8.25</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E43" s="11" t="s">
-        <v>245</v>
-      </c>
-      <c r="G43" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="H43" s="5">
-        <f>H41*H42</f>
-        <v>1</v>
-      </c>
-      <c r="I43" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="J43" s="11"/>
-      <c r="L43" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="M43" s="5">
-        <f>SS303FatigueStrength</f>
-        <v>34800</v>
-      </c>
-      <c r="N43" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="O43" s="11"/>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="B44" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="C44" s="5">
-        <f>C42/2</f>
-        <v>400</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="E44" s="11"/>
-      <c r="G44" s="10" t="s">
-        <v>242</v>
-      </c>
-      <c r="H44" s="27">
-        <f>SQRT((6*C48)/H43)</f>
-        <v>0.75429802945611568</v>
-      </c>
-      <c r="I44" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="J44" s="11"/>
-      <c r="L44" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="M44" s="5">
-        <v>5</v>
-      </c>
-      <c r="N44" s="5"/>
-      <c r="O44" s="11"/>
-    </row>
-    <row r="45" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B45" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="C45" s="5">
-        <f>C44*C43/2</f>
-        <v>1650</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="E45" s="11"/>
-      <c r="G45" s="23"/>
-      <c r="H45" s="34"/>
-      <c r="I45" s="34"/>
-      <c r="J45" s="30"/>
-      <c r="L45" s="10" t="s">
-        <v>247</v>
-      </c>
-      <c r="M45" s="5">
-        <f>M41*M44*FS/(M43*M42)</f>
-        <v>0.22988505747126436</v>
-      </c>
-      <c r="N45" s="5"/>
-      <c r="O45" s="11"/>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="B46" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C46" s="5">
-        <v>2</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E46" s="11"/>
-      <c r="L46" s="10" t="s">
-        <v>248</v>
-      </c>
-      <c r="M46" s="5">
-        <f>2*SQRT((M41*FS/H42)/M43)</f>
-        <v>0.30323921743156135</v>
-      </c>
-      <c r="N46" s="5"/>
-      <c r="O46" s="11"/>
-    </row>
-    <row r="47" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B47" s="10" t="s">
-        <v>241</v>
-      </c>
-      <c r="C47" s="5">
-        <f>SS303FatigueStrength</f>
-        <v>34800</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E47" s="11"/>
-      <c r="L47" s="23" t="s">
-        <v>177</v>
-      </c>
-      <c r="M47" s="34">
-        <f>3/8</f>
-        <v>0.375</v>
-      </c>
-      <c r="N47" s="34"/>
-      <c r="O47" s="30"/>
-    </row>
-    <row r="48" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B48" s="23" t="s">
-        <v>240</v>
-      </c>
-      <c r="C48" s="34">
-        <f>C45*C46/C47</f>
+      <c r="C33" s="34">
+        <f>C30*C31/C32</f>
         <v>9.4827586206896547E-2</v>
       </c>
-      <c r="D48" s="34" t="s">
-        <v>341</v>
-      </c>
-      <c r="E48" s="30"/>
-    </row>
-    <row r="53" spans="2:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B53" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B54" s="31" t="s">
-        <v>268</v>
-      </c>
-      <c r="C54" s="32"/>
-      <c r="D54" s="32"/>
-      <c r="E54" s="33"/>
-      <c r="G54" s="31" t="s">
-        <v>267</v>
-      </c>
-      <c r="H54" s="32"/>
-      <c r="I54" s="32"/>
-      <c r="J54" s="33"/>
-      <c r="L54" s="31" t="s">
-        <v>249</v>
-      </c>
-      <c r="M54" s="32"/>
-      <c r="N54" s="32"/>
-      <c r="O54" s="33"/>
-    </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B55" s="10"/>
-      <c r="C55" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E55" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="G55" s="10"/>
-      <c r="H55" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I55" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="J55" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="L55" s="10"/>
-      <c r="M55" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="N55" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="O55" s="11" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="56" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B56" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="C56" s="5">
-        <f>AppliedForceNormal</f>
-        <v>600</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="E56" s="11"/>
-      <c r="G56" s="10" t="s">
-        <v>238</v>
-      </c>
-      <c r="H56" s="27">
-        <v>0.5</v>
-      </c>
-      <c r="I56" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="J56" s="11"/>
-      <c r="L56" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="M56" s="5">
-        <f>C56</f>
-        <v>600</v>
-      </c>
-      <c r="N56" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="O56" s="11"/>
-    </row>
-    <row r="57" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B57" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="C57" s="5">
-        <f>MachineWidth-0.25</f>
-        <v>8.25</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E57" s="11" t="s">
-        <v>245</v>
-      </c>
-      <c r="G57" s="10" t="s">
-        <v>239</v>
-      </c>
-      <c r="H57" s="27">
-        <v>2</v>
-      </c>
-      <c r="I57" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J57" s="11"/>
-      <c r="L57" s="10" t="s">
-        <v>246</v>
-      </c>
-      <c r="M57" s="5">
-        <f>H58</f>
-        <v>1</v>
-      </c>
-      <c r="N57" s="5"/>
-      <c r="O57" s="11"/>
-    </row>
-    <row r="58" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B58" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="C58" s="5">
-        <f>C56/2</f>
-        <v>300</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="E58" s="11"/>
-      <c r="G58" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="H58" s="5">
-        <f>H56*H57</f>
-        <v>1</v>
-      </c>
-      <c r="I58" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="J58" s="11"/>
-      <c r="L58" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="M58" s="5">
-        <f>SS303FatigueStrength</f>
-        <v>34800</v>
-      </c>
-      <c r="N58" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="O58" s="11"/>
-    </row>
-    <row r="59" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B59" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="C59" s="5">
-        <f>C58*C57/2</f>
-        <v>1237.5</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="E59" s="11"/>
-      <c r="G59" s="10" t="s">
-        <v>242</v>
-      </c>
-      <c r="H59" s="27">
-        <f>SQRT((6*C62)/H58)</f>
-        <v>0.65324125553353907</v>
-      </c>
-      <c r="I59" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="J59" s="11"/>
-      <c r="L59" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="M59" s="5">
-        <v>5</v>
-      </c>
-      <c r="N59" s="5"/>
-      <c r="O59" s="11"/>
-    </row>
-    <row r="60" spans="2:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B60" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C60" s="5">
-        <v>2</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E60" s="11"/>
-      <c r="G60" s="23"/>
-      <c r="H60" s="34"/>
-      <c r="I60" s="34"/>
-      <c r="J60" s="30"/>
-      <c r="L60" s="10" t="s">
-        <v>247</v>
-      </c>
-      <c r="M60" s="5">
-        <f>M56*M59*FS/(M58*M57)</f>
-        <v>0.17241379310344829</v>
-      </c>
-      <c r="N60" s="5"/>
-      <c r="O60" s="11"/>
-    </row>
-    <row r="61" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B61" s="10" t="s">
-        <v>241</v>
-      </c>
-      <c r="C61" s="5">
-        <f>SS303FatigueStrength</f>
-        <v>34800</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E61" s="11"/>
-      <c r="L61" s="10" t="s">
-        <v>248</v>
-      </c>
-      <c r="M61" s="5">
-        <f>2*SQRT((M56*FS/H57)/M58)</f>
-        <v>0.26261286571944509</v>
-      </c>
-      <c r="N61" s="5"/>
-      <c r="O61" s="11"/>
-    </row>
-    <row r="62" spans="2:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B62" s="23" t="s">
-        <v>240</v>
-      </c>
-      <c r="C62" s="34">
-        <f>C59*C60/C61</f>
-        <v>7.1120689655172417E-2</v>
-      </c>
-      <c r="D62" s="34" t="s">
-        <v>341</v>
-      </c>
-      <c r="E62" s="30"/>
-      <c r="L62" s="23" t="s">
-        <v>177</v>
-      </c>
-      <c r="M62" s="34">
-        <f>3/8</f>
-        <v>0.375</v>
-      </c>
-      <c r="N62" s="34"/>
-      <c r="O62" s="30"/>
-    </row>
-    <row r="67" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B68" s="31"/>
-      <c r="C68" s="32"/>
-      <c r="D68" s="32"/>
-      <c r="E68" s="33"/>
-    </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B69" s="10"/>
-      <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
-      <c r="E69" s="11"/>
-    </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B70" s="10"/>
-      <c r="C70" s="5"/>
-      <c r="D70" s="5"/>
-      <c r="E70" s="11"/>
-    </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B71" s="10"/>
-      <c r="C71" s="5"/>
-      <c r="D71" s="5"/>
-      <c r="E71" s="11"/>
-    </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B72" s="10"/>
-      <c r="C72" s="5"/>
-      <c r="D72" s="5"/>
-      <c r="E72" s="11"/>
-    </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B73" s="10"/>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
-      <c r="E73" s="11"/>
-    </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B74" s="10"/>
-      <c r="C74" s="5"/>
-      <c r="D74" s="5"/>
-      <c r="E74" s="11"/>
-    </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B75" s="10"/>
-      <c r="C75" s="5"/>
-      <c r="D75" s="5"/>
-      <c r="E75" s="11"/>
-    </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B76" s="10"/>
-      <c r="C76" s="5"/>
-      <c r="D76" s="5"/>
-      <c r="E76" s="11"/>
-    </row>
-    <row r="77" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B77" s="23"/>
-      <c r="C77" s="34"/>
-      <c r="D77" s="34"/>
-      <c r="E77" s="30"/>
+      <c r="D33" s="34" t="s">
+        <v>338</v>
+      </c>
+      <c r="E33" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5932,12 +5302,12 @@
   <sheetData>
     <row r="2" spans="3:12" x14ac:dyDescent="0.45">
       <c r="J2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="3" spans="3:12" x14ac:dyDescent="0.45">
       <c r="D3" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4" spans="3:12" x14ac:dyDescent="0.45">
@@ -5951,15 +5321,15 @@
         <v>5</v>
       </c>
       <c r="J4" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="K4" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="5" spans="3:12" x14ac:dyDescent="0.45">
       <c r="D5" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="E5">
         <f>AppliedForceNormal/E6</f>
@@ -5970,12 +5340,12 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="K5" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6" spans="3:12" x14ac:dyDescent="0.45">
       <c r="D6" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -5983,18 +5353,18 @@
     </row>
     <row r="7" spans="3:12" x14ac:dyDescent="0.45">
       <c r="D7" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="E7">
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="8" spans="3:12" x14ac:dyDescent="0.45">
       <c r="D8" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="E8">
         <v>0.5</v>
@@ -6005,10 +5375,10 @@
     </row>
     <row r="9" spans="3:12" x14ac:dyDescent="0.45">
       <c r="C9" s="3" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D9" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="E9">
         <v>0.4</v>
@@ -6020,7 +5390,7 @@
     <row r="10" spans="3:12" x14ac:dyDescent="0.45">
       <c r="C10" s="3"/>
       <c r="D10" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="E10">
         <f>(E9+E8)/2</f>
@@ -6030,15 +5400,15 @@
         <v>71</v>
       </c>
       <c r="J10" s="45" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="K10" s="45" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="11" spans="3:12" x14ac:dyDescent="0.45">
       <c r="D11" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -6047,7 +5417,7 @@
         <v>71</v>
       </c>
       <c r="J11" s="45" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="K11" s="45">
         <f>'Motor Sizing Calcs'!L8</f>
@@ -6059,19 +5429,19 @@
     </row>
     <row r="12" spans="3:12" x14ac:dyDescent="0.45">
       <c r="C12" s="3" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D12" t="s">
         <v>116</v>
       </c>
       <c r="E12" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="F12" t="s">
         <v>11</v>
       </c>
       <c r="J12" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="K12">
         <v>3.73</v>
@@ -6082,7 +5452,7 @@
     </row>
     <row r="13" spans="3:12" x14ac:dyDescent="0.45">
       <c r="D13" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="E13">
         <v>18100</v>
@@ -6091,7 +5461,7 @@
         <v>13</v>
       </c>
       <c r="J13" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="K13">
         <f>E10/2</f>
@@ -6103,7 +5473,7 @@
     </row>
     <row r="14" spans="3:12" x14ac:dyDescent="0.45">
       <c r="D14" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="E14">
         <v>27700</v>
@@ -6112,7 +5482,7 @@
         <v>13</v>
       </c>
       <c r="J14" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="K14">
         <f>K12-K13</f>
@@ -6124,16 +5494,16 @@
     </row>
     <row r="15" spans="3:12" x14ac:dyDescent="0.45">
       <c r="D15" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="J15" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="K15">
         <f>K12+K13</f>
@@ -6145,85 +5515,85 @@
     </row>
     <row r="16" spans="3:12" x14ac:dyDescent="0.45">
       <c r="D16" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="E16">
         <f>E15*J5</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="F16" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="J16" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="K16">
         <f>($K$11*$K$15)</f>
         <v>865.73516370337461</v>
       </c>
       <c r="L16" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="17" spans="4:12" x14ac:dyDescent="0.45">
       <c r="D17" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="E17">
         <f>E7*E16</f>
         <v>3.333333333333333</v>
       </c>
       <c r="F17" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="J17" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="K17">
         <f>(-1*$K$11*-1*$K$15)</f>
         <v>865.73516370337461</v>
       </c>
       <c r="L17" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="18" spans="4:12" x14ac:dyDescent="0.45">
       <c r="J18" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="K18">
         <f>($K$11*-1*$K$14)</f>
         <v>-767.23179488756705</v>
       </c>
       <c r="L18" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="19" spans="4:12" x14ac:dyDescent="0.45">
       <c r="D19" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="E19">
         <f>PI()*E8*(E7/2)</f>
         <v>7.8539816339744828</v>
       </c>
       <c r="F19" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="J19" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="K19">
         <f>(-1*$K$11*$K$14)</f>
         <v>-767.23179488756705</v>
       </c>
       <c r="L19" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="20" spans="4:12" x14ac:dyDescent="0.45">
       <c r="D20" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="E20">
         <f>((E8/2)^2*PI())-((E9/2)^2*PI())</f>
@@ -6237,7 +5607,7 @@
         <v>197.00673763161512</v>
       </c>
       <c r="L20" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="21" spans="4:12" x14ac:dyDescent="0.45">
@@ -6246,12 +5616,12 @@
         <v>16.417228135967928</v>
       </c>
       <c r="L21" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="22" spans="4:12" x14ac:dyDescent="0.45">
       <c r="D22" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="E22">
         <f>E19*E16</f>
@@ -6264,7 +5634,7 @@
         <v>114.59155902616466</v>
       </c>
       <c r="J23" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="K23">
         <f>K20/MachineWidth</f>
@@ -6280,7 +5650,7 @@
         <v>4244.1318157838768</v>
       </c>
       <c r="J24" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="K24">
         <f>K23*MachineHeight/MachineWidth</f>
@@ -6352,11 +5722,11 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B7" s="5"/>
       <c r="D7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E7" cm="1">
         <f t="array" ref="E7">(MMH-PTIH)*(((WCID/2)^2)-((WPRT/2)^2))/((2*((WCID/2)^2))-((WPRT/2)^2))</f>
@@ -6368,14 +5738,14 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B8" s="5">
         <f>1.5</f>
         <v>1.5</v>
       </c>
       <c r="D8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E8">
         <f>(WPRT^2)*E7/((WCID^2)-(WPRT^2))</f>
@@ -6384,7 +5754,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B9" s="5">
         <v>1.67</v>
@@ -6392,13 +5762,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B10" s="5">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E10">
         <f>E7+E8+B9+B11</f>
@@ -6407,31 +5777,31 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B11" s="5">
         <v>1.67</v>
       </c>
       <c r="D11" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E11">
         <f>E7+E8+B11</f>
         <v>8.8979339669834925</v>
       </c>
       <c r="F11" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B12" s="5">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E12">
         <f>E7+E8+B10</f>
@@ -6440,7 +5810,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="5" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="B13" s="5">
         <v>0.5</v>
@@ -6452,7 +5822,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B15" s="5">
         <f>SUM(B8:B13)</f>

</xml_diff>